<commit_message>
Fin du TD4 (avec des données manquantes)
Correction des erreurs commises lors de la première partie du TD4 et ajout d'une partie des questions de la seconde partie (avec deux questions manquantes)
</commit_message>
<xml_diff>
--- a/Controle de gestion - TD4.xlsx
+++ b/Controle de gestion - TD4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amtti\Documents\Université\Controle de gestion\M1---Controle-de-gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91AB967-23CF-44B3-B45D-354CE37707E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE8B0A7-5D0F-4A08-ADC3-B50F3963FBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{E93606DE-3904-4879-9FF7-DAF90B90E367}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="102">
   <si>
     <t>Exercice 1</t>
   </si>
@@ -253,10 +253,99 @@
     <t>5. Pas pour un nouveau produit, à moins qu'il soit très similaire au produit étudié.</t>
   </si>
   <si>
-    <t>Chiffres faux, voir photos</t>
-  </si>
-  <si>
     <t>Je n'ai pas réussi à prendre la fin de la correction. Je corrigerai ça plus tard.</t>
+  </si>
+  <si>
+    <t>Document non fini, voir photos du 23/01/2024</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>Exercice 3</t>
+  </si>
+  <si>
+    <t>Volume des ventes trimestrielles (en milliers de tubes Y)</t>
+  </si>
+  <si>
+    <t>N-3</t>
+  </si>
+  <si>
+    <t>N-2</t>
+  </si>
+  <si>
+    <t>N-1</t>
+  </si>
+  <si>
+    <t>2e trimestre</t>
+  </si>
+  <si>
+    <t>Ventes (xy)</t>
+  </si>
+  <si>
+    <t>Xi^2</t>
+  </si>
+  <si>
+    <t>Tendance</t>
+  </si>
+  <si>
+    <t>Coef saisonnier</t>
+  </si>
+  <si>
+    <t>Moyennes</t>
+  </si>
+  <si>
+    <t>Trimestres</t>
+  </si>
+  <si>
+    <t>Prévisions</t>
+  </si>
+  <si>
+    <t>Exercice 4</t>
+  </si>
+  <si>
+    <t>Xi (xi-x_)</t>
+  </si>
+  <si>
+    <t>Yi (yi-y_)</t>
+  </si>
+  <si>
+    <t>Yi^2</t>
+  </si>
+  <si>
+    <t>Coef saisonnier ajusté</t>
+  </si>
+  <si>
+    <t>Coefs ajustés</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>Valeurs observées</t>
+  </si>
+  <si>
+    <t>Valeurs ajustées</t>
+  </si>
+  <si>
+    <t>Indices
+saisonniers
+(Vo/Va)</t>
+  </si>
+  <si>
+    <t>trimestres</t>
+  </si>
+  <si>
+    <t>coefs moyens</t>
+  </si>
+  <si>
+    <t>Prévisions année N</t>
+  </si>
+  <si>
+    <t>On obtient normalement ces valeurs dans la question 2</t>
+  </si>
+  <si>
+    <t>Pas fini</t>
   </si>
 </sst>
 </file>
@@ -421,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -437,9 +526,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -450,18 +536,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2970,10 +3065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29CACBE-41B4-4F0D-BDDD-8C9E237DAFD9}">
-  <dimension ref="A1:V114"/>
+  <dimension ref="A1:V234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="H204" sqref="H204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2990,13 +3085,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -3760,56 +3855,56 @@
       </c>
     </row>
     <row r="68" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A68" s="10" t="s">
+      <c r="A68" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B68" s="11" t="s">
+      <c r="B68" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="C68" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D68" s="11" t="s">
+      <c r="D68" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E68" s="12" t="s">
+      <c r="E68" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A69" s="13">
+      <c r="A69" s="12">
         <v>1</v>
       </c>
-      <c r="B69" s="14">
+      <c r="B69">
         <v>110</v>
       </c>
-      <c r="C69" s="15"/>
-      <c r="D69" s="16">
+      <c r="C69" s="6"/>
+      <c r="D69" s="8">
         <f>$I$55*A69+$I$57</f>
         <v>104.27113970588235</v>
       </c>
-      <c r="E69" s="17">
+      <c r="E69" s="13">
         <f>B69/D69</f>
         <v>1.0549419552742691</v>
       </c>
-      <c r="G69" s="22" t="s">
+      <c r="G69" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="H69" s="22"/>
+      <c r="H69" s="20"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A70" s="13">
+      <c r="A70" s="12">
         <v>2</v>
       </c>
-      <c r="B70" s="14">
+      <c r="B70">
         <v>90</v>
       </c>
-      <c r="C70" s="15"/>
-      <c r="D70" s="16">
+      <c r="C70" s="6"/>
+      <c r="D70" s="8">
         <f t="shared" ref="D70:D88" si="4">$I$55*A70+$I$57</f>
         <v>106.70312499999999</v>
       </c>
-      <c r="E70" s="17">
+      <c r="E70" s="13">
         <f t="shared" ref="E70:E88" si="5">B70/D70</f>
         <v>0.84346170742422033</v>
       </c>
@@ -3822,21 +3917,21 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A71" s="13">
+      <c r="A71" s="12">
         <v>3</v>
       </c>
-      <c r="B71" s="14">
+      <c r="B71">
         <v>75</v>
       </c>
-      <c r="C71" s="14">
+      <c r="C71">
         <f>1/4*(1/2*B69+B70+B71+B72+1/2*B73)</f>
         <v>108.75</v>
       </c>
-      <c r="D71" s="16">
+      <c r="D71" s="8">
         <f t="shared" si="4"/>
         <v>109.13511029411764</v>
       </c>
-      <c r="E71" s="17">
+      <c r="E71" s="13">
         <f t="shared" si="5"/>
         <v>0.68722155315439748</v>
       </c>
@@ -3849,21 +3944,21 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A72" s="13">
+      <c r="A72" s="12">
         <v>4</v>
       </c>
-      <c r="B72" s="14">
+      <c r="B72">
         <v>150</v>
       </c>
-      <c r="C72" s="14">
+      <c r="C72">
         <f t="shared" ref="C72:C86" si="7">1/4*(1/2*B70+B71+B72+B73+1/2*B74)</f>
         <v>112.5</v>
       </c>
-      <c r="D72" s="16">
+      <c r="D72" s="8">
         <f t="shared" si="4"/>
         <v>111.56709558823529</v>
       </c>
-      <c r="E72" s="17">
+      <c r="E72" s="13">
         <f t="shared" si="5"/>
         <v>1.3444824319314579</v>
       </c>
@@ -3876,21 +3971,21 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A73" s="13">
+      <c r="A73" s="12">
         <v>5</v>
       </c>
-      <c r="B73" s="14">
+      <c r="B73">
         <v>130</v>
       </c>
-      <c r="C73" s="14">
+      <c r="C73">
         <f t="shared" si="7"/>
         <v>113.125</v>
       </c>
-      <c r="D73" s="16">
+      <c r="D73" s="8">
         <f t="shared" si="4"/>
         <v>113.99908088235293</v>
       </c>
-      <c r="E73" s="17">
+      <c r="E73" s="13">
         <f t="shared" si="5"/>
         <v>1.1403600712725046</v>
       </c>
@@ -3903,21 +3998,21 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A74" s="13">
+      <c r="A74" s="12">
         <v>6</v>
       </c>
-      <c r="B74" s="14">
+      <c r="B74">
         <v>100</v>
       </c>
-      <c r="C74" s="14">
+      <c r="C74">
         <f t="shared" si="7"/>
         <v>116.25</v>
       </c>
-      <c r="D74" s="16">
+      <c r="D74" s="8">
         <f t="shared" si="4"/>
         <v>116.43106617647058</v>
       </c>
-      <c r="E74" s="17">
+      <c r="E74" s="13">
         <f t="shared" si="5"/>
         <v>0.85887730211482749</v>
       </c>
@@ -3930,21 +4025,21 @@
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A75" s="13">
+      <c r="A75" s="12">
         <v>7</v>
       </c>
-      <c r="B75" s="14">
+      <c r="B75">
         <v>70</v>
       </c>
-      <c r="C75" s="14">
+      <c r="C75">
         <f t="shared" si="7"/>
         <v>120.375</v>
       </c>
-      <c r="D75" s="16">
+      <c r="D75" s="8">
         <f t="shared" si="4"/>
         <v>118.86305147058823</v>
       </c>
-      <c r="E75" s="17">
+      <c r="E75" s="13">
         <f t="shared" si="5"/>
         <v>0.5889130317112965</v>
       </c>
@@ -3953,21 +4048,21 @@
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A76" s="13">
+      <c r="A76" s="12">
         <v>8</v>
       </c>
-      <c r="B76" s="14">
+      <c r="B76">
         <v>180</v>
       </c>
-      <c r="C76" s="14">
+      <c r="C76">
         <f t="shared" si="7"/>
         <v>121.25</v>
       </c>
-      <c r="D76" s="16">
+      <c r="D76" s="8">
         <f t="shared" si="4"/>
         <v>121.29503676470587</v>
       </c>
-      <c r="E76" s="17">
+      <c r="E76" s="13">
         <f t="shared" si="5"/>
         <v>1.4839848752358511</v>
       </c>
@@ -3979,49 +4074,49 @@
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A77" s="13">
+      <c r="A77" s="12">
         <v>9</v>
       </c>
-      <c r="B77" s="14">
+      <c r="B77">
         <v>133</v>
       </c>
-      <c r="C77" s="14">
+      <c r="C77">
         <f t="shared" si="7"/>
         <v>124.25</v>
       </c>
-      <c r="D77" s="16">
+      <c r="D77" s="8">
         <f t="shared" si="4"/>
         <v>123.72702205882352</v>
       </c>
-      <c r="E77" s="17">
+      <c r="E77" s="13">
         <f t="shared" si="5"/>
         <v>1.0749470712773466</v>
       </c>
-      <c r="G77" s="22" t="s">
+      <c r="G77" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="H77" s="22"/>
-      <c r="I77" s="22"/>
+      <c r="H77" s="20"/>
+      <c r="I77" s="20"/>
       <c r="K77" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A78" s="13">
+      <c r="A78" s="12">
         <v>10</v>
       </c>
-      <c r="B78" s="14">
+      <c r="B78">
         <v>104</v>
       </c>
-      <c r="C78" s="14">
+      <c r="C78">
         <f t="shared" si="7"/>
         <v>125.625</v>
       </c>
-      <c r="D78" s="16">
+      <c r="D78" s="8">
         <f t="shared" si="4"/>
         <v>126.15900735294116</v>
       </c>
-      <c r="E78" s="17">
+      <c r="E78" s="13">
         <f t="shared" si="5"/>
         <v>0.82435651787470599</v>
       </c>
@@ -4038,21 +4133,21 @@
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A79" s="13">
+      <c r="A79" s="12">
         <v>11</v>
       </c>
-      <c r="B79" s="14">
+      <c r="B79">
         <v>90</v>
       </c>
-      <c r="C79" s="14">
+      <c r="C79">
         <f t="shared" si="7"/>
         <v>126.625</v>
       </c>
-      <c r="D79" s="16">
+      <c r="D79" s="8">
         <f t="shared" si="4"/>
         <v>128.59099264705881</v>
       </c>
-      <c r="E79" s="17">
+      <c r="E79" s="13">
         <f t="shared" si="5"/>
         <v>0.69989350068259637</v>
       </c>
@@ -4069,21 +4164,21 @@
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A80" s="13">
+      <c r="A80" s="12">
         <v>12</v>
       </c>
-      <c r="B80" s="14">
+      <c r="B80">
         <v>171</v>
       </c>
-      <c r="C80" s="14">
+      <c r="C80">
         <f t="shared" si="7"/>
         <v>130.125</v>
       </c>
-      <c r="D80" s="16">
+      <c r="D80" s="8">
         <f t="shared" si="4"/>
         <v>131.02297794117646</v>
       </c>
-      <c r="E80" s="17">
+      <c r="E80" s="13">
         <f t="shared" si="5"/>
         <v>1.3051145889598956</v>
       </c>
@@ -4100,21 +4195,21 @@
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A81" s="13">
+      <c r="A81" s="12">
         <v>13</v>
       </c>
-      <c r="B81" s="14">
+      <c r="B81">
         <v>150</v>
       </c>
-      <c r="C81" s="14">
+      <c r="C81">
         <f t="shared" si="7"/>
         <v>132.75</v>
       </c>
-      <c r="D81" s="16">
+      <c r="D81" s="8">
         <f t="shared" si="4"/>
         <v>133.45496323529412</v>
       </c>
-      <c r="E81" s="17">
+      <c r="E81" s="13">
         <f t="shared" si="5"/>
         <v>1.1239746830212329</v>
       </c>
@@ -4131,135 +4226,135 @@
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A82" s="13">
+      <c r="A82" s="12">
         <v>14</v>
       </c>
-      <c r="B82" s="14">
+      <c r="B82">
         <v>115</v>
       </c>
-      <c r="C82" s="14">
+      <c r="C82">
         <f t="shared" si="7"/>
         <v>137.625</v>
       </c>
-      <c r="D82" s="16">
+      <c r="D82" s="8">
         <f t="shared" si="4"/>
         <v>135.88694852941177</v>
       </c>
-      <c r="E82" s="17">
+      <c r="E82" s="13">
         <f t="shared" si="5"/>
         <v>0.84629172444113765</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A83" s="13">
+      <c r="A83" s="12">
         <v>15</v>
       </c>
-      <c r="B83" s="14">
+      <c r="B83">
         <v>100</v>
       </c>
-      <c r="C83" s="14">
+      <c r="C83">
         <f t="shared" si="7"/>
         <v>140.625</v>
       </c>
-      <c r="D83" s="16">
+      <c r="D83" s="8">
         <f t="shared" si="4"/>
         <v>138.31893382352939</v>
       </c>
-      <c r="E83" s="17">
+      <c r="E83" s="13">
         <f t="shared" si="5"/>
         <v>0.72296682193619566</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A84" s="13">
+      <c r="A84" s="12">
         <v>16</v>
       </c>
-      <c r="B84" s="14">
+      <c r="B84">
         <v>200</v>
       </c>
-      <c r="C84" s="14">
+      <c r="C84">
         <f t="shared" si="7"/>
         <v>140.625</v>
       </c>
-      <c r="D84" s="16">
+      <c r="D84" s="8">
         <f t="shared" si="4"/>
         <v>140.75091911764704</v>
       </c>
-      <c r="E84" s="17">
+      <c r="E84" s="13">
         <f t="shared" si="5"/>
         <v>1.4209498684184751</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A85" s="13">
+      <c r="A85" s="12">
         <v>17</v>
       </c>
-      <c r="B85" s="14">
+      <c r="B85">
         <v>145</v>
       </c>
-      <c r="C85" s="14">
+      <c r="C85">
         <f t="shared" si="7"/>
         <v>141.875</v>
       </c>
-      <c r="D85" s="16">
+      <c r="D85" s="8">
         <f t="shared" si="4"/>
         <v>143.1829044117647</v>
       </c>
-      <c r="E85" s="17">
+      <c r="E85" s="13">
         <f t="shared" si="5"/>
         <v>1.0126907300539854</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A86" s="13">
+      <c r="A86" s="12">
         <v>18</v>
       </c>
-      <c r="B86" s="14">
+      <c r="B86">
         <v>120</v>
       </c>
-      <c r="C86" s="14">
+      <c r="C86">
         <f t="shared" si="7"/>
         <v>145.625</v>
       </c>
-      <c r="D86" s="16">
+      <c r="D86" s="8">
         <f t="shared" si="4"/>
         <v>145.61488970588235</v>
       </c>
-      <c r="E86" s="17">
+      <c r="E86" s="13">
         <f t="shared" si="5"/>
         <v>0.82409154889571989</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A87" s="13">
+      <c r="A87" s="12">
         <v>19</v>
       </c>
-      <c r="B87" s="14">
+      <c r="B87">
         <v>105</v>
       </c>
-      <c r="C87" s="15"/>
-      <c r="D87" s="16">
+      <c r="C87" s="6"/>
+      <c r="D87" s="8">
         <f t="shared" si="4"/>
         <v>148.046875</v>
       </c>
-      <c r="E87" s="17">
+      <c r="E87" s="13">
         <f t="shared" si="5"/>
         <v>0.70923482849604225</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A88" s="18">
+      <c r="A88" s="14">
         <v>20</v>
       </c>
-      <c r="B88" s="19">
+      <c r="B88" s="15">
         <v>225</v>
       </c>
-      <c r="C88" s="20"/>
-      <c r="D88" s="16">
+      <c r="C88" s="16"/>
+      <c r="D88" s="8">
         <f t="shared" si="4"/>
         <v>150.47886029411762</v>
       </c>
-      <c r="E88" s="21">
+      <c r="E88" s="17">
         <f t="shared" si="5"/>
         <v>1.4952266355568318</v>
       </c>
@@ -4402,7 +4497,7 @@
       </c>
       <c r="J99">
         <f>E105</f>
-        <v>4996.2</v>
+        <v>4936.8</v>
       </c>
       <c r="M99">
         <v>12</v>
@@ -4428,11 +4523,11 @@
       </c>
       <c r="S99">
         <f>N99-$N$105</f>
-        <v>-377.59999999999991</v>
+        <v>-375.40000000000009</v>
       </c>
       <c r="T99">
         <f>R99*S99</f>
-        <v>1736.96</v>
+        <v>1726.8400000000011</v>
       </c>
       <c r="U99">
         <f>R99^2</f>
@@ -4440,7 +4535,7 @@
       </c>
       <c r="V99">
         <f>S99^2</f>
-        <v>142581.75999999992</v>
+        <v>140925.16000000006</v>
       </c>
     </row>
     <row r="100" spans="1:22" x14ac:dyDescent="0.35">
@@ -4456,11 +4551,11 @@
       </c>
       <c r="D100">
         <f>B100-$B$106</f>
-        <v>-377.59999999999991</v>
+        <v>-375.40000000000009</v>
       </c>
       <c r="E100">
         <f>C100*D100</f>
-        <v>1736.96</v>
+        <v>1726.8400000000011</v>
       </c>
       <c r="F100">
         <f>(A100-$A$106)^2</f>
@@ -4468,14 +4563,14 @@
       </c>
       <c r="G100">
         <f>(B100-$B$106)^2</f>
-        <v>142581.75999999992</v>
+        <v>140925.16000000006</v>
       </c>
       <c r="I100" t="s">
         <v>60</v>
       </c>
       <c r="J100">
         <f>SQRT(F105*G105)</f>
-        <v>5074.8940323912184</v>
+        <v>5025.4221554014748</v>
       </c>
       <c r="M100">
         <v>14</v>
@@ -4501,11 +4596,11 @@
       </c>
       <c r="S100">
         <f t="shared" ref="S100:S103" si="12">N100-$N$105</f>
-        <v>-137.59999999999991</v>
+        <v>-135.40000000000009</v>
       </c>
       <c r="T100">
         <f t="shared" ref="T100:T103" si="13">R100*S100</f>
-        <v>357.75999999999993</v>
+        <v>352.04000000000042</v>
       </c>
       <c r="U100">
         <f t="shared" ref="U100:U103" si="14">R100^2</f>
@@ -4513,7 +4608,7 @@
       </c>
       <c r="V100">
         <f t="shared" ref="V100:V103" si="15">S100^2</f>
-        <v>18933.759999999977</v>
+        <v>18333.160000000025</v>
       </c>
     </row>
     <row r="101" spans="1:22" x14ac:dyDescent="0.35">
@@ -4529,11 +4624,11 @@
       </c>
       <c r="D101">
         <f t="shared" ref="D101:D104" si="17">B101-$B$106</f>
-        <v>-137.59999999999991</v>
+        <v>-135.40000000000009</v>
       </c>
       <c r="E101">
         <f t="shared" ref="E101:E104" si="18">C101*D101</f>
-        <v>357.75999999999993</v>
+        <v>352.04000000000042</v>
       </c>
       <c r="F101">
         <f t="shared" ref="F101:F104" si="19">(A101-$A$106)^2</f>
@@ -4541,14 +4636,14 @@
       </c>
       <c r="G101">
         <f t="shared" ref="G101:G104" si="20">(B101-$B$106)^2</f>
-        <v>18933.759999999977</v>
+        <v>18333.160000000025</v>
       </c>
       <c r="I101" t="s">
         <v>61</v>
       </c>
       <c r="J101">
         <f>J99/J100</f>
-        <v>0.98449346293953277</v>
+        <v>0.98236523168382561</v>
       </c>
       <c r="M101">
         <v>15</v>
@@ -4574,11 +4669,11 @@
       </c>
       <c r="S101">
         <f t="shared" si="12"/>
-        <v>-100.59999999999991</v>
+        <v>-98.400000000000091</v>
       </c>
       <c r="T101">
         <f t="shared" si="13"/>
-        <v>160.96</v>
+        <v>157.44000000000028</v>
       </c>
       <c r="U101">
         <f t="shared" si="14"/>
@@ -4586,7 +4681,7 @@
       </c>
       <c r="V101">
         <f t="shared" si="15"/>
-        <v>10120.359999999982</v>
+        <v>9682.5600000000177</v>
       </c>
     </row>
     <row r="102" spans="1:22" x14ac:dyDescent="0.35">
@@ -4602,11 +4697,11 @@
       </c>
       <c r="D102">
         <f t="shared" si="17"/>
-        <v>-100.59999999999991</v>
+        <v>-98.400000000000091</v>
       </c>
       <c r="E102">
         <f t="shared" si="18"/>
-        <v>160.96</v>
+        <v>157.44000000000028</v>
       </c>
       <c r="F102">
         <f t="shared" si="19"/>
@@ -4614,7 +4709,7 @@
       </c>
       <c r="G102">
         <f t="shared" si="20"/>
-        <v>10120.359999999982</v>
+        <v>9682.5600000000177</v>
       </c>
       <c r="M102">
         <v>20</v>
@@ -4640,11 +4735,11 @@
       </c>
       <c r="S102">
         <f t="shared" si="12"/>
-        <v>292.40000000000009</v>
+        <v>294.59999999999991</v>
       </c>
       <c r="T102">
         <f t="shared" si="13"/>
-        <v>994.15999999999985</v>
+        <v>1001.6399999999993</v>
       </c>
       <c r="U102">
         <f t="shared" si="14"/>
@@ -4652,7 +4747,7 @@
       </c>
       <c r="V102">
         <f t="shared" si="15"/>
-        <v>85497.760000000053</v>
+        <v>86789.159999999945</v>
       </c>
     </row>
     <row r="103" spans="1:22" x14ac:dyDescent="0.35">
@@ -4668,11 +4763,11 @@
       </c>
       <c r="D103">
         <f t="shared" si="17"/>
-        <v>292.40000000000009</v>
+        <v>294.59999999999991</v>
       </c>
       <c r="E103">
         <f t="shared" si="18"/>
-        <v>994.15999999999985</v>
+        <v>1001.6399999999993</v>
       </c>
       <c r="F103">
         <f t="shared" si="19"/>
@@ -4680,17 +4775,17 @@
       </c>
       <c r="G103">
         <f t="shared" si="20"/>
-        <v>85497.760000000053</v>
+        <v>86789.159999999945</v>
       </c>
       <c r="M103">
         <v>22</v>
       </c>
       <c r="N103">
-        <v>2021</v>
+        <v>2010</v>
       </c>
       <c r="O103">
         <f t="shared" si="8"/>
-        <v>44462</v>
+        <v>44220</v>
       </c>
       <c r="P103">
         <f t="shared" si="9"/>
@@ -4698,7 +4793,7 @@
       </c>
       <c r="Q103">
         <f t="shared" si="10"/>
-        <v>4084441</v>
+        <v>4040100</v>
       </c>
       <c r="R103">
         <f t="shared" si="11"/>
@@ -4706,11 +4801,11 @@
       </c>
       <c r="S103">
         <f t="shared" si="12"/>
-        <v>323.40000000000009</v>
+        <v>314.59999999999991</v>
       </c>
       <c r="T103">
         <f t="shared" si="13"/>
-        <v>1746.3600000000001</v>
+        <v>1698.839999999999</v>
       </c>
       <c r="U103">
         <f t="shared" si="14"/>
@@ -4718,7 +4813,7 @@
       </c>
       <c r="V103">
         <f t="shared" si="15"/>
-        <v>104587.56000000006</v>
+        <v>98973.159999999945</v>
       </c>
     </row>
     <row r="104" spans="1:22" x14ac:dyDescent="0.35">
@@ -4726,7 +4821,7 @@
         <v>22</v>
       </c>
       <c r="B104">
-        <v>2021</v>
+        <v>2010</v>
       </c>
       <c r="C104">
         <f t="shared" si="16"/>
@@ -4734,11 +4829,11 @@
       </c>
       <c r="D104">
         <f t="shared" si="17"/>
-        <v>323.40000000000009</v>
+        <v>314.59999999999991</v>
       </c>
       <c r="E104">
         <f t="shared" si="18"/>
-        <v>1746.3600000000001</v>
+        <v>1698.839999999999</v>
       </c>
       <c r="F104">
         <f t="shared" si="19"/>
@@ -4746,7 +4841,7 @@
       </c>
       <c r="G104">
         <f t="shared" si="20"/>
-        <v>104587.56000000006</v>
+        <v>98973.159999999945</v>
       </c>
       <c r="M104" s="7">
         <f>SUM(M99:M103)</f>
@@ -4754,11 +4849,11 @@
       </c>
       <c r="N104" s="7">
         <f>SUM(N99:N103)</f>
-        <v>8488</v>
+        <v>8477</v>
       </c>
       <c r="O104" s="7">
         <f t="shared" ref="O104:U104" si="21">SUM(O99:O103)</f>
-        <v>145897</v>
+        <v>145655</v>
       </c>
       <c r="P104" s="7">
         <f t="shared" si="21"/>
@@ -4766,7 +4861,7 @@
       </c>
       <c r="Q104" s="7">
         <f t="shared" si="21"/>
-        <v>14770950</v>
+        <v>14726609</v>
       </c>
       <c r="R104" s="7">
         <f t="shared" si="21"/>
@@ -4774,18 +4869,15 @@
       </c>
       <c r="S104" s="7">
         <f t="shared" si="21"/>
-        <v>4.5474735088646412E-13</v>
+        <v>-4.5474735088646412E-13</v>
       </c>
       <c r="T104" s="7">
         <f t="shared" si="21"/>
-        <v>4996.2</v>
+        <v>4936.8</v>
       </c>
       <c r="U104" s="7">
         <f t="shared" si="21"/>
         <v>71.2</v>
-      </c>
-      <c r="V104" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="105" spans="1:22" x14ac:dyDescent="0.35">
@@ -4795,19 +4887,19 @@
       </c>
       <c r="B105" s="7">
         <f>SUM(B100:B104)</f>
-        <v>8488</v>
-      </c>
-      <c r="C105" s="23">
+        <v>8477</v>
+      </c>
+      <c r="C105" s="18">
         <f t="shared" ref="C105:G105" si="22">SUM(C100:C104)</f>
         <v>-7.1054273576010019E-15</v>
       </c>
-      <c r="D105" s="23">
+      <c r="D105" s="18">
         <f t="shared" si="22"/>
-        <v>4.5474735088646412E-13</v>
+        <v>-4.5474735088646412E-13</v>
       </c>
       <c r="E105" s="7">
         <f t="shared" si="22"/>
-        <v>4996.2</v>
+        <v>4936.8</v>
       </c>
       <c r="F105" s="7">
         <f t="shared" si="22"/>
@@ -4815,7 +4907,7 @@
       </c>
       <c r="G105" s="7">
         <f t="shared" si="22"/>
-        <v>361721.2</v>
+        <v>354703.2</v>
       </c>
       <c r="M105">
         <f>AVERAGE(M99:M103)</f>
@@ -4823,7 +4915,7 @@
       </c>
       <c r="N105">
         <f>AVERAGE(N99:N103)</f>
-        <v>1697.6</v>
+        <v>1695.4</v>
       </c>
     </row>
     <row r="106" spans="1:22" x14ac:dyDescent="0.35">
@@ -4833,7 +4925,12 @@
       </c>
       <c r="B106">
         <f>AVERAGE(B100:B104)</f>
-        <v>1697.6</v>
+        <v>1695.4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="P107" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="108" spans="1:22" x14ac:dyDescent="0.35">
@@ -4853,12 +4950,1544 @@
     </row>
     <row r="112" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A118" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B121" t="s">
+        <v>76</v>
+      </c>
+      <c r="C121" t="s">
+        <v>77</v>
+      </c>
+      <c r="D121" t="s">
+        <v>78</v>
+      </c>
+      <c r="E121" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>37</v>
+      </c>
+      <c r="B122">
+        <v>524</v>
+      </c>
+      <c r="C122">
+        <v>532</v>
+      </c>
+      <c r="D122">
+        <v>556</v>
+      </c>
+      <c r="E122">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>79</v>
+      </c>
+      <c r="B123">
+        <v>378</v>
+      </c>
+      <c r="C123">
+        <v>418</v>
+      </c>
+      <c r="D123">
+        <v>426</v>
+      </c>
+      <c r="E123">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>41</v>
+      </c>
+      <c r="B124">
+        <v>354</v>
+      </c>
+      <c r="C124">
+        <v>378</v>
+      </c>
+      <c r="D124">
+        <v>394</v>
+      </c>
+      <c r="E124">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>39</v>
+      </c>
+      <c r="B125">
+        <v>636</v>
+      </c>
+      <c r="C125">
+        <v>692</v>
+      </c>
+      <c r="D125">
+        <v>716</v>
+      </c>
+      <c r="E125">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B126" s="7">
+        <f t="shared" ref="B126:E126" si="23">AVERAGE(B122:B125)</f>
+        <v>473</v>
+      </c>
+      <c r="C126" s="7">
+        <f t="shared" si="23"/>
+        <v>505</v>
+      </c>
+      <c r="D126" s="7">
+        <f t="shared" si="23"/>
+        <v>523</v>
+      </c>
+      <c r="E126" s="7">
+        <f t="shared" si="23"/>
+        <v>575</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>11</v>
+      </c>
+      <c r="B128" t="s">
+        <v>80</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D128" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129">
+        <v>1</v>
+      </c>
+      <c r="B129">
+        <v>524</v>
+      </c>
+      <c r="C129" s="6"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130">
+        <v>2</v>
+      </c>
+      <c r="B130">
+        <v>378</v>
+      </c>
+      <c r="C130" s="6"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131">
+        <v>3</v>
+      </c>
+      <c r="B131">
+        <v>354</v>
+      </c>
+      <c r="C131">
+        <f>1/4*(1/2*B129+B130+B131+B132+1/2*B133)</f>
+        <v>474</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132">
+        <v>4</v>
+      </c>
+      <c r="B132">
+        <v>636</v>
+      </c>
+      <c r="C132">
+        <f t="shared" ref="C132:C142" si="24">1/4*(1/2*B130+B131+B132+B133+1/2*B134)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133">
+        <v>5</v>
+      </c>
+      <c r="B133">
+        <v>532</v>
+      </c>
+      <c r="C133">
+        <f t="shared" si="24"/>
+        <v>488</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134">
+        <v>6</v>
+      </c>
+      <c r="B134">
+        <v>418</v>
+      </c>
+      <c r="C134">
+        <f t="shared" si="24"/>
+        <v>498</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135">
+        <v>7</v>
+      </c>
+      <c r="B135">
+        <v>378</v>
+      </c>
+      <c r="C135">
+        <f t="shared" si="24"/>
+        <v>508</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136">
+        <v>8</v>
+      </c>
+      <c r="B136">
+        <v>692</v>
+      </c>
+      <c r="C136">
+        <f t="shared" si="24"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137">
+        <v>9</v>
+      </c>
+      <c r="B137">
+        <v>556</v>
+      </c>
+      <c r="C137">
+        <f t="shared" si="24"/>
+        <v>515</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138">
+        <v>10</v>
+      </c>
+      <c r="B138">
+        <v>426</v>
+      </c>
+      <c r="C138">
+        <f t="shared" si="24"/>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139">
+        <v>11</v>
+      </c>
+      <c r="B139">
+        <v>394</v>
+      </c>
+      <c r="C139">
+        <f t="shared" si="24"/>
+        <v>536</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140">
+        <v>12</v>
+      </c>
+      <c r="B140">
+        <v>716</v>
+      </c>
+      <c r="C140">
+        <f t="shared" si="24"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141">
+        <v>13</v>
+      </c>
+      <c r="B141">
+        <v>660</v>
+      </c>
+      <c r="C141">
+        <f t="shared" si="24"/>
+        <v>568</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142">
+        <v>14</v>
+      </c>
+      <c r="B142">
+        <v>482</v>
+      </c>
+      <c r="C142">
+        <f t="shared" si="24"/>
+        <v>574</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143">
+        <v>15</v>
+      </c>
+      <c r="B143">
+        <v>434</v>
+      </c>
+      <c r="C143" s="6"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144">
+        <v>16</v>
+      </c>
+      <c r="B144">
+        <v>724</v>
+      </c>
+      <c r="C144" s="6"/>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>11</v>
+      </c>
+      <c r="B149" t="s">
+        <v>80</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D149" t="s">
+        <v>83</v>
+      </c>
+      <c r="H149" t="s">
+        <v>30</v>
+      </c>
+      <c r="I149">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>1</v>
+      </c>
+      <c r="B150">
+        <v>524</v>
+      </c>
+      <c r="C150" s="6"/>
+      <c r="H150" t="s">
+        <v>32</v>
+      </c>
+      <c r="I150">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <v>2</v>
+      </c>
+      <c r="B151">
+        <v>378</v>
+      </c>
+      <c r="C151" s="6"/>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <v>3</v>
+      </c>
+      <c r="B152">
+        <v>354</v>
+      </c>
+      <c r="C152">
+        <f>1/4*(1/2*B150+B151+B152+B153+1/2*B154)</f>
+        <v>474</v>
+      </c>
+      <c r="D152">
+        <f>B152/C152</f>
+        <v>0.74683544303797467</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A153">
+        <v>4</v>
+      </c>
+      <c r="B153">
+        <v>636</v>
+      </c>
+      <c r="C153">
+        <f t="shared" ref="C153:C163" si="25">1/4*(1/2*B151+B152+B153+B154+1/2*B155)</f>
+        <v>480</v>
+      </c>
+      <c r="D153">
+        <f>B153/C153</f>
+        <v>1.325</v>
+      </c>
+      <c r="H153" t="s">
+        <v>85</v>
+      </c>
+      <c r="I153" t="s">
+        <v>84</v>
+      </c>
+      <c r="K153" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A154">
+        <v>5</v>
+      </c>
+      <c r="B154">
+        <v>532</v>
+      </c>
+      <c r="C154">
+        <f t="shared" si="25"/>
+        <v>488</v>
+      </c>
+      <c r="D154">
+        <f>B154/C154</f>
+        <v>1.0901639344262295</v>
+      </c>
+      <c r="H154">
+        <v>3</v>
+      </c>
+      <c r="I154" s="21">
+        <f>(C152+C156+C160)/3</f>
+        <v>506</v>
+      </c>
+      <c r="J154">
+        <f>(D152+D156+D160)/3</f>
+        <v>0.74200151936420744</v>
+      </c>
+      <c r="K154">
+        <f>J154*$J$159</f>
+        <v>0.74074264504961418</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A155">
+        <v>6</v>
+      </c>
+      <c r="B155">
+        <v>418</v>
+      </c>
+      <c r="C155">
+        <f t="shared" si="25"/>
+        <v>498</v>
+      </c>
+      <c r="D155">
+        <f>B155/C155</f>
+        <v>0.8393574297188755</v>
+      </c>
+      <c r="H155">
+        <v>4</v>
+      </c>
+      <c r="I155" s="21">
+        <f t="shared" ref="I155:I157" si="26">(C153+C157+C161)/3</f>
+        <v>516</v>
+      </c>
+      <c r="J155">
+        <f>(D153+D157+D161)/3</f>
+        <v>1.3214440947242208</v>
+      </c>
+      <c r="K155">
+        <f t="shared" ref="K155:K157" si="27">J155*$J$159</f>
+        <v>1.3192021424025535</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A156">
+        <v>7</v>
+      </c>
+      <c r="B156">
+        <v>378</v>
+      </c>
+      <c r="C156">
+        <f t="shared" si="25"/>
+        <v>508</v>
+      </c>
+      <c r="D156">
+        <f>B156/C156</f>
+        <v>0.74409448818897639</v>
+      </c>
+      <c r="H156">
+        <v>1</v>
+      </c>
+      <c r="I156" s="21">
+        <f t="shared" si="26"/>
+        <v>523.66666666666663</v>
+      </c>
+      <c r="J156">
+        <f>(D154+D158+D162)/3</f>
+        <v>1.1105824719658606</v>
+      </c>
+      <c r="K156">
+        <f t="shared" si="27"/>
+        <v>1.1086982659208471</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A157">
+        <v>8</v>
+      </c>
+      <c r="B157">
+        <v>692</v>
+      </c>
+      <c r="C157">
+        <f t="shared" si="25"/>
+        <v>512</v>
+      </c>
+      <c r="D157">
+        <f>B157/C157</f>
+        <v>1.3515625</v>
+      </c>
+      <c r="H157">
+        <v>2</v>
+      </c>
+      <c r="I157" s="21">
+        <f t="shared" si="26"/>
+        <v>530.66666666666663</v>
+      </c>
+      <c r="J157">
+        <f>(D155+D159+D163)/3</f>
+        <v>0.83276981776834846</v>
+      </c>
+      <c r="K157">
+        <f t="shared" si="27"/>
+        <v>0.83135694662698567</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A158">
+        <v>9</v>
+      </c>
+      <c r="B158">
+        <v>556</v>
+      </c>
+      <c r="C158">
+        <f t="shared" si="25"/>
+        <v>515</v>
+      </c>
+      <c r="D158">
+        <f>B158/C158</f>
+        <v>1.0796116504854369</v>
+      </c>
+      <c r="J158">
+        <f>SUM(J154:J157)</f>
+        <v>4.0067979038226369</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A159">
+        <v>10</v>
+      </c>
+      <c r="B159">
+        <v>426</v>
+      </c>
+      <c r="C159">
+        <f t="shared" si="25"/>
+        <v>520</v>
+      </c>
+      <c r="D159">
+        <f>B159/C159</f>
+        <v>0.81923076923076921</v>
+      </c>
+      <c r="H159" t="s">
+        <v>91</v>
+      </c>
+      <c r="J159">
+        <f>4/J158</f>
+        <v>0.99830340736273437</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A160">
+        <v>11</v>
+      </c>
+      <c r="B160">
+        <v>394</v>
+      </c>
+      <c r="C160">
+        <f t="shared" si="25"/>
+        <v>536</v>
+      </c>
+      <c r="D160">
+        <f>B160/C160</f>
+        <v>0.7350746268656716</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A161">
+        <v>12</v>
+      </c>
+      <c r="B161">
+        <v>716</v>
+      </c>
+      <c r="C161">
+        <f t="shared" si="25"/>
+        <v>556</v>
+      </c>
+      <c r="D161">
+        <f>B161/C161</f>
+        <v>1.2877697841726619</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A162">
+        <v>13</v>
+      </c>
+      <c r="B162">
+        <v>660</v>
+      </c>
+      <c r="C162">
+        <f t="shared" si="25"/>
+        <v>568</v>
+      </c>
+      <c r="D162">
+        <f>B162/C162</f>
+        <v>1.1619718309859155</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A163">
+        <v>14</v>
+      </c>
+      <c r="B163">
+        <v>482</v>
+      </c>
+      <c r="C163">
+        <f t="shared" si="25"/>
+        <v>574</v>
+      </c>
+      <c r="D163">
+        <f>B163/C163</f>
+        <v>0.83972125435540068</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A164">
+        <v>15</v>
+      </c>
+      <c r="B164">
+        <v>434</v>
+      </c>
+      <c r="C164" s="6"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A165">
+        <v>16</v>
+      </c>
+      <c r="B165">
+        <v>724</v>
+      </c>
+      <c r="C165" s="6"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>85</v>
+      </c>
+      <c r="B172" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A173">
+        <v>17</v>
+      </c>
+      <c r="B173">
+        <f>($I$149*A173+$I$150)*K156</f>
+        <v>679.63203700947929</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A174">
+        <v>18</v>
+      </c>
+      <c r="B174">
+        <f>($I$149*A174+$I$150)*K157</f>
+        <v>517.10402080198514</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A175">
+        <v>19</v>
+      </c>
+      <c r="B175">
+        <f>($I$149*A175+$I$150)*K154</f>
+        <v>467.40860902630652</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A176">
+        <v>20</v>
+      </c>
+      <c r="B176">
+        <f>($I$149*A176+$I$150)*K155</f>
+        <v>844.28937113763425</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B177" s="7">
+        <f>SUM(B173:B176)</f>
+        <v>2508.4340379754053</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A178" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A180" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B180" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C180" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D180" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E180" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F180" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="G180" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="I180" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A181" s="12">
+        <v>1</v>
+      </c>
+      <c r="B181">
+        <v>610</v>
+      </c>
+      <c r="C181">
+        <f>A181-$A$187</f>
+        <v>-2</v>
+      </c>
+      <c r="D181">
+        <f>B181-$B$187</f>
+        <v>-354</v>
+      </c>
+      <c r="E181">
+        <f>C181*D181</f>
+        <v>708</v>
+      </c>
+      <c r="F181">
+        <f>C181^2</f>
+        <v>4</v>
+      </c>
+      <c r="G181">
+        <f>D181^2</f>
+        <v>125316</v>
+      </c>
+      <c r="I181" t="s">
+        <v>59</v>
+      </c>
+      <c r="J181">
+        <f>E186</f>
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A182" s="12">
+        <v>2</v>
+      </c>
+      <c r="B182">
+        <v>818</v>
+      </c>
+      <c r="C182">
+        <f>A182-$A$187</f>
+        <v>-1</v>
+      </c>
+      <c r="D182">
+        <f>B182-$B$187</f>
+        <v>-146</v>
+      </c>
+      <c r="E182">
+        <f t="shared" ref="E182:E200" si="28">C182*D182</f>
+        <v>146</v>
+      </c>
+      <c r="F182">
+        <f t="shared" ref="F182:F200" si="29">C182^2</f>
+        <v>1</v>
+      </c>
+      <c r="G182">
+        <f t="shared" ref="G182:G200" si="30">D182^2</f>
+        <v>21316</v>
+      </c>
+      <c r="I182" t="s">
+        <v>60</v>
+      </c>
+      <c r="J182">
+        <f>SQRT(F186*G186)</f>
+        <v>1683.6804922549884</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A183" s="12">
+        <v>3</v>
+      </c>
+      <c r="B183">
+        <v>943</v>
+      </c>
+      <c r="C183">
+        <f>A183-$A$187</f>
+        <v>0</v>
+      </c>
+      <c r="D183">
+        <f>B183-$B$187</f>
+        <v>-21</v>
+      </c>
+      <c r="E183">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="F183">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="G183">
+        <f t="shared" si="30"/>
+        <v>441</v>
+      </c>
+      <c r="I183" t="s">
+        <v>61</v>
+      </c>
+      <c r="J183">
+        <f>J181/J182</f>
+        <v>0.98237165994883224</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A184" s="12">
+        <v>4</v>
+      </c>
+      <c r="B184">
+        <v>1206</v>
+      </c>
+      <c r="C184">
+        <f>A184-$A$187</f>
+        <v>1</v>
+      </c>
+      <c r="D184">
+        <f>B184-$B$187</f>
+        <v>242</v>
+      </c>
+      <c r="E184">
+        <f t="shared" si="28"/>
+        <v>242</v>
+      </c>
+      <c r="F184">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="G184">
+        <f t="shared" si="30"/>
+        <v>58564</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A185" s="12">
+        <v>5</v>
+      </c>
+      <c r="B185">
+        <v>1243</v>
+      </c>
+      <c r="C185">
+        <f>A185-$A$187</f>
+        <v>2</v>
+      </c>
+      <c r="D185">
+        <f>B185-$B$187</f>
+        <v>279</v>
+      </c>
+      <c r="E185">
+        <f t="shared" si="28"/>
+        <v>558</v>
+      </c>
+      <c r="F185">
+        <f t="shared" si="29"/>
+        <v>4</v>
+      </c>
+      <c r="G185">
+        <f t="shared" si="30"/>
+        <v>77841</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A186" s="22">
+        <f>SUM(A181:A185)</f>
+        <v>15</v>
+      </c>
+      <c r="B186" s="22">
+        <f>SUM(B181:B185)</f>
+        <v>4820</v>
+      </c>
+      <c r="C186" s="22">
+        <f>SUM(C181:C185)</f>
+        <v>0</v>
+      </c>
+      <c r="D186" s="22">
+        <f>SUM(D181:D185)</f>
+        <v>0</v>
+      </c>
+      <c r="E186" s="22">
+        <f>SUM(E181:E185)</f>
+        <v>1654</v>
+      </c>
+      <c r="F186" s="22">
+        <f>SUM(F181:F185)</f>
+        <v>10</v>
+      </c>
+      <c r="G186" s="22">
+        <f>SUM(G181:G185)</f>
+        <v>283478</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A187">
+        <f>AVERAGE(A181:A185)</f>
+        <v>3</v>
+      </c>
+      <c r="B187">
+        <f>AVERAGE(B181:B185)</f>
+        <v>964</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A188" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A189" s="12"/>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A190" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B190" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A191" s="12">
+        <v>1</v>
+      </c>
+      <c r="B191">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A192" s="12">
+        <v>2</v>
+      </c>
+      <c r="B192">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A193" s="12">
+        <v>3</v>
+      </c>
+      <c r="B193">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A194" s="12">
+        <v>4</v>
+      </c>
+      <c r="B194">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A195" s="12">
+        <v>5</v>
+      </c>
+      <c r="B195">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A196" s="12">
+        <v>6</v>
+      </c>
+      <c r="B196">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A197" s="12">
+        <v>7</v>
+      </c>
+      <c r="B197">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A198" s="12">
+        <v>8</v>
+      </c>
+      <c r="B198">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A199" s="12">
+        <v>9</v>
+      </c>
+      <c r="B199">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A200" s="14">
+        <v>10</v>
+      </c>
+      <c r="B200">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A201" s="24">
+        <v>11</v>
+      </c>
+      <c r="B201">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A202" s="24">
+        <v>12</v>
+      </c>
+      <c r="B202">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A203" s="24">
+        <v>13</v>
+      </c>
+      <c r="B203">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A204" s="24">
+        <v>14</v>
+      </c>
+      <c r="B204">
+        <v>275</v>
+      </c>
+      <c r="G204" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A205" s="24">
+        <v>15</v>
+      </c>
+      <c r="B205">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A206" s="24">
+        <v>16</v>
+      </c>
+      <c r="B206">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A207" s="24">
+        <v>17</v>
+      </c>
+      <c r="B207">
+        <v>158</v>
+      </c>
+      <c r="G207" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A208" s="24">
+        <v>18</v>
+      </c>
+      <c r="B208">
+        <v>312</v>
+      </c>
+      <c r="G208" t="s">
+        <v>30</v>
+      </c>
+      <c r="H208">
+        <v>10.37</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A209" s="24">
+        <v>19</v>
+      </c>
+      <c r="B209">
+        <v>641</v>
+      </c>
+      <c r="G209" t="s">
+        <v>32</v>
+      </c>
+      <c r="H209">
+        <v>132.12</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A210" s="24">
+        <v>20</v>
+      </c>
+      <c r="B210">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A214" t="s">
+        <v>85</v>
+      </c>
+      <c r="B214" t="s">
+        <v>94</v>
+      </c>
+      <c r="C214" t="s">
+        <v>95</v>
+      </c>
+      <c r="D214" s="25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A215" s="12">
+        <v>1</v>
+      </c>
+      <c r="B215">
+        <v>92</v>
+      </c>
+      <c r="C215">
+        <v>142.49</v>
+      </c>
+      <c r="D215">
+        <f>B215/C215</f>
+        <v>0.64565934451540452</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A216" s="12">
+        <v>2</v>
+      </c>
+      <c r="B216">
+        <v>151</v>
+      </c>
+      <c r="C216">
+        <v>152.86000000000001</v>
+      </c>
+      <c r="D216">
+        <f t="shared" ref="D216:D234" si="31">B216/C216</f>
+        <v>0.98783200314012809</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A217" s="12">
+        <v>3</v>
+      </c>
+      <c r="B217">
+        <v>306</v>
+      </c>
+      <c r="C217">
+        <v>163.22999999999999</v>
+      </c>
+      <c r="D217">
+        <f t="shared" si="31"/>
+        <v>1.8746553942290021</v>
+      </c>
+      <c r="G217" t="s">
+        <v>97</v>
+      </c>
+      <c r="H217" t="s">
+        <v>98</v>
+      </c>
+      <c r="I217" t="s">
+        <v>92</v>
+      </c>
+      <c r="J217" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A218" s="12">
+        <v>4</v>
+      </c>
+      <c r="B218">
+        <v>61</v>
+      </c>
+      <c r="C218">
+        <v>173.6</v>
+      </c>
+      <c r="D218">
+        <f t="shared" si="31"/>
+        <v>0.35138248847926268</v>
+      </c>
+      <c r="G218">
+        <v>21</v>
+      </c>
+      <c r="H218">
+        <f>(D215+D219+D223+D227+D231)/5</f>
+        <v>0.66933316466998394</v>
+      </c>
+      <c r="I218">
+        <f>H218*$H$223</f>
+        <v>0.67060437626040015</v>
+      </c>
+      <c r="J218">
+        <f>($H$208*G218+$H$209)*I218</f>
+        <v>234.63776520975139</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A219" s="12">
+        <v>5</v>
+      </c>
+      <c r="B219">
+        <v>125</v>
+      </c>
+      <c r="C219">
+        <v>183.97</v>
+      </c>
+      <c r="D219">
+        <f t="shared" si="31"/>
+        <v>0.67945860738163832</v>
+      </c>
+      <c r="G219">
+        <v>22</v>
+      </c>
+      <c r="H219">
+        <f t="shared" ref="H219:H221" si="32">(D216+D220+D224+D228+D232)/5</f>
+        <v>0.99732628666938827</v>
+      </c>
+      <c r="I219">
+        <f t="shared" ref="I219:I221" si="33">H219*$H$223</f>
+        <v>0.9992204296791195</v>
+      </c>
+      <c r="J219">
+        <f t="shared" ref="J219:J221" si="34">($H$208*G219+$H$209)*I219</f>
+        <v>359.97915199619956</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A220" s="12">
+        <v>6</v>
+      </c>
+      <c r="B220">
+        <v>203</v>
+      </c>
+      <c r="C220">
+        <v>194.34</v>
+      </c>
+      <c r="D220">
+        <f t="shared" si="31"/>
+        <v>1.0445610785221775</v>
+      </c>
+      <c r="G220">
+        <v>23</v>
+      </c>
+      <c r="H220">
+        <f t="shared" si="32"/>
+        <v>1.9029096414506406</v>
+      </c>
+      <c r="I220">
+        <f t="shared" si="33"/>
+        <v>1.9065236873688935</v>
+      </c>
+      <c r="J220">
+        <f t="shared" si="34"/>
+        <v>706.61487424953305</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A221" s="12">
+        <v>7</v>
+      </c>
+      <c r="B221">
+        <v>395</v>
+      </c>
+      <c r="C221">
+        <v>204.71</v>
+      </c>
+      <c r="D221">
+        <f t="shared" si="31"/>
+        <v>1.9295588881832837</v>
+      </c>
+      <c r="G221">
+        <v>24</v>
+      </c>
+      <c r="H221">
+        <f t="shared" si="32"/>
+        <v>0.42284842409226542</v>
+      </c>
+      <c r="I221">
+        <f t="shared" si="33"/>
+        <v>0.42365150669158702</v>
+      </c>
+      <c r="J221">
+        <f t="shared" si="34"/>
+        <v>161.41122404949465</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A222" s="12">
+        <v>8</v>
+      </c>
+      <c r="B222">
+        <v>95</v>
+      </c>
+      <c r="C222">
+        <v>215.08</v>
+      </c>
+      <c r="D222">
+        <f t="shared" si="31"/>
+        <v>0.44169611307420492</v>
+      </c>
+      <c r="H222" s="7">
+        <f t="shared" ref="H222:I222" si="35">SUM(H218:H221)</f>
+        <v>3.992417516882278</v>
+      </c>
+      <c r="I222" s="7">
+        <f t="shared" si="35"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A223" s="12">
+        <v>9</v>
+      </c>
+      <c r="B223">
+        <v>146</v>
+      </c>
+      <c r="C223">
+        <v>225.45</v>
+      </c>
+      <c r="D223">
+        <f t="shared" si="31"/>
+        <v>0.64759370148591711</v>
+      </c>
+      <c r="H223">
+        <f>4/H222</f>
+        <v>1.0018992209821891</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A224" s="14">
+        <v>10</v>
+      </c>
+      <c r="B224">
+        <v>232</v>
+      </c>
+      <c r="C224">
+        <v>235.82</v>
+      </c>
+      <c r="D224">
+        <f t="shared" si="31"/>
+        <v>0.98380120430837081</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A225" s="24">
+        <v>11</v>
+      </c>
+      <c r="B225">
+        <v>442</v>
+      </c>
+      <c r="C225">
+        <v>246.19</v>
+      </c>
+      <c r="D225">
+        <f t="shared" si="31"/>
+        <v>1.795361306308136</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A226" s="24">
+        <v>12</v>
+      </c>
+      <c r="B226">
+        <v>123</v>
+      </c>
+      <c r="C226">
+        <v>256.56</v>
+      </c>
+      <c r="D226">
+        <f t="shared" si="31"/>
+        <v>0.47942001870907391</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A227" s="24">
+        <v>13</v>
+      </c>
+      <c r="B227">
+        <v>230</v>
+      </c>
+      <c r="C227">
+        <v>266.93</v>
+      </c>
+      <c r="D227">
+        <f t="shared" si="31"/>
+        <v>0.86164912149252615</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A228" s="24">
+        <v>14</v>
+      </c>
+      <c r="B228">
+        <v>275</v>
+      </c>
+      <c r="C228">
+        <v>277.3</v>
+      </c>
+      <c r="D228">
+        <f t="shared" si="31"/>
+        <v>0.99170573386224303</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A229" s="24">
+        <v>15</v>
+      </c>
+      <c r="B229">
+        <v>566</v>
+      </c>
+      <c r="C229">
+        <v>287.67</v>
+      </c>
+      <c r="D229">
+        <f t="shared" si="31"/>
+        <v>1.9675322418048458</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A230" s="24">
+        <v>16</v>
+      </c>
+      <c r="B230">
+        <v>135</v>
+      </c>
+      <c r="C230">
+        <v>298.04000000000002</v>
+      </c>
+      <c r="D230">
+        <f t="shared" si="31"/>
+        <v>0.45295933431754126</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A231" s="24">
+        <v>17</v>
+      </c>
+      <c r="B231">
+        <v>158</v>
+      </c>
+      <c r="C231">
+        <v>308.41000000000003</v>
+      </c>
+      <c r="D231">
+        <f t="shared" si="31"/>
+        <v>0.51230504847443337</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A232" s="24">
+        <v>18</v>
+      </c>
+      <c r="B232">
+        <v>312</v>
+      </c>
+      <c r="C232">
+        <v>318.77999999999997</v>
+      </c>
+      <c r="D232">
+        <f t="shared" si="31"/>
+        <v>0.97873141351402226</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A233" s="24">
+        <v>19</v>
+      </c>
+      <c r="B233">
+        <v>641</v>
+      </c>
+      <c r="C233">
+        <v>329.15</v>
+      </c>
+      <c r="D233">
+        <f t="shared" si="31"/>
+        <v>1.9474403767279358</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A234" s="24">
+        <v>20</v>
+      </c>
+      <c r="B234">
+        <v>132</v>
+      </c>
+      <c r="C234">
+        <v>339.52</v>
+      </c>
+      <c r="D234">
+        <f t="shared" si="31"/>
+        <v>0.38878416588124415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>